<commit_message>
Unit assignment is added
</commit_message>
<xml_diff>
--- a/api/df.xlsx
+++ b/api/df.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
   <si>
     <t xml:space="preserve">Site</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">cap-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max-grad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min-fraction</t>
   </si>
   <si>
     <t xml:space="preserve">inv-cost</t>
@@ -92,17 +86,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -187,7 +181,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -200,11 +194,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,15 +210,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,10 +313,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,31 +343,25 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>0</v>
@@ -388,34 +372,28 @@
       <c r="E2" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="n">
+      <c r="F2" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="9" t="n">
+      <c r="G2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="K2" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L2" s="8" t="n">
+      <c r="I2" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J2" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>0</v>
@@ -426,34 +404,28 @@
       <c r="E3" s="6" t="n">
         <v>60000</v>
       </c>
-      <c r="F3" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="n">
+      <c r="F3" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="9" t="n">
+      <c r="G3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="K3" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L3" s="8" t="n">
+      <c r="I3" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J3" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="n">
         <v>0</v>
@@ -464,34 +436,28 @@
       <c r="E4" s="6" t="n">
         <v>80000</v>
       </c>
-      <c r="F4" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="n">
+      <c r="F4" s="6" t="n">
         <v>450000</v>
       </c>
-      <c r="I4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9" t="n">
+      <c r="G4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="n">
         <v>1.6</v>
       </c>
-      <c r="K4" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L4" s="8" t="n">
+      <c r="I4" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J4" s="8" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>0</v>
@@ -502,34 +468,28 @@
       <c r="E5" s="6" t="n">
         <v>5000</v>
       </c>
-      <c r="F5" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="n">
+      <c r="F5" s="6" t="n">
         <v>875000</v>
       </c>
-      <c r="I5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="9" t="n">
+      <c r="G5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7" t="n">
         <v>1.4</v>
       </c>
-      <c r="K5" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L5" s="8" t="n">
+      <c r="I5" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J5" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>0</v>
@@ -540,34 +500,28 @@
       <c r="E6" s="6" t="n">
         <v>13000</v>
       </c>
-      <c r="F6" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6" t="n">
+      <c r="F6" s="6" t="n">
         <v>1500000</v>
       </c>
-      <c r="I6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L6" s="8" t="n">
+      <c r="G6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J6" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>0</v>
@@ -578,34 +532,28 @@
       <c r="E7" s="6" t="n">
         <v>160000</v>
       </c>
-      <c r="F7" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="n">
+      <c r="F7" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I7" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L7" s="8" t="n">
+      <c r="G7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J7" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>0</v>
@@ -616,34 +564,28 @@
       <c r="E8" s="6" t="n">
         <v>1400</v>
       </c>
-      <c r="F8" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G8" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6" t="n">
+      <c r="F8" s="6" t="n">
         <v>1600000</v>
       </c>
-      <c r="I8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L8" s="8" t="n">
+      <c r="G8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J8" s="8" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>0</v>
@@ -654,34 +596,28 @@
       <c r="E9" s="6" t="n">
         <v>100000</v>
       </c>
-      <c r="F9" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="n">
+      <c r="F9" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I9" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="9" t="n">
+      <c r="G9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="K9" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L9" s="8" t="n">
+      <c r="I9" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J9" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>0</v>
@@ -692,34 +628,28 @@
       <c r="E10" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6" t="n">
+      <c r="F10" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9" t="n">
+      <c r="G10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="K10" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L10" s="8" t="n">
+      <c r="I10" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J10" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>0</v>
@@ -730,34 +660,28 @@
       <c r="E11" s="6" t="n">
         <v>100000</v>
       </c>
-      <c r="F11" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6" t="n">
+      <c r="F11" s="6" t="n">
         <v>450000</v>
       </c>
-      <c r="I11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="9" t="n">
+      <c r="G11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7" t="n">
         <v>1.6</v>
       </c>
-      <c r="K11" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L11" s="8" t="n">
+      <c r="I11" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J11" s="8" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>0</v>
@@ -768,34 +692,28 @@
       <c r="E12" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6" t="n">
+      <c r="F12" s="6" t="n">
         <v>875000</v>
       </c>
-      <c r="I12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="9" t="n">
+      <c r="G12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7" t="n">
         <v>1.4</v>
       </c>
-      <c r="K12" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L12" s="8" t="n">
+      <c r="I12" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J12" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="6" t="n">
         <v>0</v>
@@ -806,34 +724,28 @@
       <c r="E13" s="6" t="n">
         <v>200000</v>
       </c>
-      <c r="F13" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6" t="n">
+      <c r="F13" s="6" t="n">
         <v>1500000</v>
       </c>
-      <c r="I13" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L13" s="8" t="n">
+      <c r="G13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J13" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>0</v>
@@ -844,34 +756,28 @@
       <c r="E14" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="F14" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G14" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6" t="n">
+      <c r="F14" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I14" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L14" s="8" t="n">
+      <c r="G14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J14" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="6" t="n">
         <v>0</v>
@@ -882,34 +788,28 @@
       <c r="E15" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G15" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6" t="n">
+      <c r="F15" s="6" t="n">
         <v>1600000</v>
       </c>
-      <c r="I15" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L15" s="8" t="n">
+      <c r="G15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J15" s="8" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>0</v>
@@ -920,34 +820,28 @@
       <c r="E16" s="6" t="n">
         <v>100000</v>
       </c>
-      <c r="F16" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G16" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6" t="n">
+      <c r="F16" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="9" t="n">
+      <c r="G16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="K16" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L16" s="8" t="n">
+      <c r="I16" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J16" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="6" t="n">
         <v>0</v>
@@ -958,34 +852,28 @@
       <c r="E17" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6" t="n">
+      <c r="F17" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I17" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="9" t="n">
+      <c r="G17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="K17" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L17" s="8" t="n">
+      <c r="I17" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J17" s="8" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>0</v>
@@ -996,34 +884,28 @@
       <c r="E18" s="6" t="n">
         <v>100000</v>
       </c>
-      <c r="F18" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="6" t="n">
+      <c r="F18" s="6" t="n">
         <v>450000</v>
       </c>
-      <c r="I18" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="9" t="n">
+      <c r="G18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7" t="n">
         <v>1.6</v>
       </c>
-      <c r="K18" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L18" s="8" t="n">
+      <c r="I18" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J18" s="8" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>0</v>
@@ -1034,34 +916,28 @@
       <c r="E19" s="6" t="n">
         <v>6000</v>
       </c>
-      <c r="F19" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G19" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6" t="n">
+      <c r="F19" s="6" t="n">
         <v>875000</v>
       </c>
-      <c r="I19" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="9" t="n">
+      <c r="G19" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7" t="n">
         <v>1.4</v>
       </c>
-      <c r="K19" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L19" s="8" t="n">
+      <c r="I19" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J19" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>0</v>
@@ -1072,34 +948,28 @@
       <c r="E20" s="6" t="n">
         <v>60000</v>
       </c>
-      <c r="F20" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G20" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="6" t="n">
+      <c r="F20" s="6" t="n">
         <v>1500000</v>
       </c>
-      <c r="I20" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L20" s="8" t="n">
+      <c r="G20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J20" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>0</v>
@@ -1110,34 +980,28 @@
       <c r="E21" s="6" t="n">
         <v>3000</v>
       </c>
-      <c r="F21" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G21" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="6" t="n">
+      <c r="F21" s="6" t="n">
         <v>600000</v>
       </c>
-      <c r="I21" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L21" s="8" t="n">
+      <c r="G21" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J21" s="8" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>0</v>
@@ -1148,205 +1012,194 @@
       <c r="E22" s="6" t="n">
         <v>20000</v>
       </c>
-      <c r="F22" s="7" t="n">
-        <v>1500000000000000</v>
-      </c>
-      <c r="G22" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6" t="n">
+      <c r="F22" s="6" t="n">
         <v>1600000</v>
       </c>
-      <c r="I22" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="8" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L22" s="8" t="n">
+      <c r="G22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="J22" s="8" t="n">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="F3">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="F2">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:J6 A6:E6">
+  <conditionalFormatting sqref="A6:H6">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
+  <conditionalFormatting sqref="I6">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
+  <conditionalFormatting sqref="I6">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
+  <conditionalFormatting sqref="J6">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6">
+  <conditionalFormatting sqref="J6">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:L7 A7:E7">
+  <conditionalFormatting sqref="G7:J7 A7:E7">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:L8 A8:E8">
+  <conditionalFormatting sqref="A8:J8">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13:J13 G13 B13:E13">
+  <conditionalFormatting sqref="G13:H13 B13:E13">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
+  <conditionalFormatting sqref="I13">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
+  <conditionalFormatting sqref="I13">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="J13">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="J13">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:L14 G14 B14:E14">
+  <conditionalFormatting sqref="G14:J14 B14:E14">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:L15 G15 B15:E15">
+  <conditionalFormatting sqref="G15:J15 B15:E15">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:J20 G20 B20:E20">
+  <conditionalFormatting sqref="G20:H20 B20:E20">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
+  <conditionalFormatting sqref="I20">
     <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
+  <conditionalFormatting sqref="I20">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20">
+  <conditionalFormatting sqref="J20">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20">
+  <conditionalFormatting sqref="J20">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:L21 G21 B21:E21">
+  <conditionalFormatting sqref="G21:J21 B21:E21">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:L22 G22 B22:E22">
+  <conditionalFormatting sqref="G22:J22 B22:E22">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="F7">
     <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="F13">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="F15">
     <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+  <conditionalFormatting sqref="F14">
     <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="F10">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
+  <conditionalFormatting sqref="F9">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
+  <conditionalFormatting sqref="F20">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="F22">
     <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
+  <conditionalFormatting sqref="F21">
     <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
+  <conditionalFormatting sqref="F17">
     <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
+  <conditionalFormatting sqref="F16">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="10">
+  <dataValidations count="8">
     <dataValidation allowBlank="true" operator="between" prompt="Existing power throughput capacity per process." promptTitle="Installed capacity (MW)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -1359,31 +1212,23 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Maximum allowed power gradient relative to power throughput capacity. Set value to inf or greater than 1/dt to disable it." promptTitle="Maximal power gradient (1/h)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F1" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Total investement cost for adding capacity. Is annualized in the model using the annuity factor derived from 'wacc' and 'depreciation'." promptTitle="Investment cost (€/MW)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="This value sets the minimum possible fraction of the process capacity which the process can run at." promptTitle="Minimum load fraction" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Operation independent costs for existing and new capacities per MW throughput power." promptTitle="Annual fix cost (€/MW/a)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Total investement cost for adding capacity. Is annualized in the model using the annuity factor derived from 'wacc' and 'depreciation'." promptTitle="Investment cost (€/MW)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Variable costs per throughput energy unit (MWh) produced. This includes wear and tear of moving parts, operation liquids, but excluding fuel costs, as they are included in table Commodity, column 'price'." promptTitle="Variable costs (€/MWh)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Operation independent costs for existing and new capacities per MW throughput power." promptTitle="Annual fix cost (€/MW/a)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Interest rate (%) of costs for capital after taxes. Used to calculate annuity factor for investment costs." promptTitle="Weighted average cost of capital" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Variable costs per throughput energy unit (MWh) produced. This includes wear and tear of moving parts, operation liquids, but excluding fuel costs, as they are included in table Commodity, column 'price'." promptTitle="Variable costs (€/MWh)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Interest rate (%) of costs for capital after taxes. Used to calculate annuity factor for investment costs." promptTitle="Weighted average cost of capital" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K1" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Economic lifetime (more conservative than technical lifetime) of a process investment in years (a). Used to calculate annuity factor for investment costs." promptTitle="Depreciation period (a)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L1" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Economic lifetime (more conservative than technical lifetime) of a process investment in years (a). Used to calculate annuity factor for investment costs." promptTitle="Depreciation period (a)" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>